<commit_message>
Remove pull up on sync input PE.11
</commit_message>
<xml_diff>
--- a/Schematic/Emat/BOM.xlsx
+++ b/Schematic/Emat/BOM.xlsx
@@ -14,7 +14,7 @@
   </sheets>
   <definedNames>
     <definedName name="Emat_merged_BOM" localSheetId="2">'Real Qty'!$A$1:$D$51</definedName>
-    <definedName name="Emat_merged_BOM" localSheetId="1">'Up-d Qty'!$A$2:$D$52</definedName>
+    <definedName name="Emat_merged_BOM" localSheetId="1">'Up-d Qty'!$A$5:$D$56</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="81">
   <si>
     <t>EFD25</t>
   </si>
@@ -253,6 +253,42 @@
   </si>
   <si>
     <t>EMAT Bill of Materials. Date: April 7, 2016</t>
+  </si>
+  <si>
+    <t>MP2307DN-MINI-MOD</t>
+  </si>
+  <si>
+    <t>AMS1117-3.3V-MODUL</t>
+  </si>
+  <si>
+    <t>DC/DC MODULES</t>
+  </si>
+  <si>
+    <t>DIODEs</t>
+  </si>
+  <si>
+    <t>POLARIZED CAPACITORs</t>
+  </si>
+  <si>
+    <t>HV CAPACITORs</t>
+  </si>
+  <si>
+    <t>CAPACITORs 0805</t>
+  </si>
+  <si>
+    <t>RESISTORs 2512</t>
+  </si>
+  <si>
+    <t>RESISTORs 1206</t>
+  </si>
+  <si>
+    <t>Magnet</t>
+  </si>
+  <si>
+    <t>TRANSFORMERs</t>
+  </si>
+  <si>
+    <t>INDUCTORs</t>
   </si>
 </sst>
 </file>
@@ -302,7 +338,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -394,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -403,13 +440,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -429,29 +459,42 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,594 +809,627 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="10"/>
-    <col min="6" max="6" width="9.140625" style="19"/>
-    <col min="7" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="9.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="19" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="7"/>
+    <col min="6" max="6" width="9.140625" style="14"/>
+    <col min="7" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="21" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:6" s="23" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A1" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="22"/>
-    </row>
-    <row r="2" spans="1:6" s="14" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A2" s="16" t="s">
+      <c r="F1" s="24"/>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" ht="12" customHeight="1">
+      <c r="A2" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:6" s="9" customFormat="1" ht="12" customHeight="1">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:6" s="9" customFormat="1" ht="12" customHeight="1">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="1:6" s="18" customFormat="1" ht="12" customHeight="1">
+      <c r="A5" s="17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A3" s="11">
-        <v>2</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="12" t="s">
+    <row r="6" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A6" s="8">
+        <v>2</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="18"/>
-    </row>
-    <row r="4" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A4" s="11">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11" t="s">
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A7" s="8">
+        <v>2</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C7" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="18"/>
-    </row>
-    <row r="5" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A5" s="11">
-        <v>2</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A8" s="8">
+        <v>2</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="18"/>
-    </row>
-    <row r="6" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A6" s="11">
-        <v>2</v>
-      </c>
-      <c r="B6" s="11" t="s">
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A9" s="8">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C9" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="18"/>
-    </row>
-    <row r="7" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A7" s="11">
-        <v>2</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A10" s="8">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C10" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="18"/>
-    </row>
-    <row r="8" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A8" s="11">
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A11" s="8">
         <v>4</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C11" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="18"/>
-    </row>
-    <row r="9" spans="1:6" s="13" customFormat="1" ht="12">
-      <c r="A9" s="17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A10" s="11">
-        <v>2</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="1:6" s="16" customFormat="1" ht="12">
+      <c r="A12" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A13" s="8">
+        <v>2</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C13" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="18"/>
-    </row>
-    <row r="11" spans="1:6" s="14" customFormat="1" ht="12">
-      <c r="A11" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A12" s="11">
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:6" s="18" customFormat="1" ht="12">
+      <c r="A14" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A15" s="8">
         <v>4</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="18"/>
-    </row>
-    <row r="13" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A13" s="11">
-        <v>2</v>
-      </c>
-      <c r="B13" s="11" t="s">
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A16" s="8">
+        <v>2</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C16" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="18"/>
-    </row>
-    <row r="14" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A14" s="11">
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A17" s="8">
         <v>4</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C17" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="18"/>
-    </row>
-    <row r="15" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A15" s="11">
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A18" s="8">
         <v>4</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C18" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="18"/>
-    </row>
-    <row r="16" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A16" s="11">
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A19" s="8">
         <v>4</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C19" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="18"/>
-    </row>
-    <row r="17" spans="1:6" s="14" customFormat="1" ht="12">
-      <c r="A17" s="16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A18" s="11">
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="1:6" s="18" customFormat="1" ht="12">
+      <c r="A20" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A21" s="8">
         <v>4</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="18"/>
-    </row>
-    <row r="19" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A19" s="11">
+      <c r="F21" s="13"/>
+    </row>
+    <row r="22" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A22" s="8">
         <v>4</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="18"/>
-    </row>
-    <row r="20" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A20" s="11">
-        <v>2</v>
-      </c>
-      <c r="B20" s="11" t="s">
+      <c r="F22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A23" s="8">
+        <v>2</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="18"/>
-    </row>
-    <row r="21" spans="1:6" s="14" customFormat="1" ht="12">
-      <c r="A21" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A22" s="11">
+      <c r="F23" s="13"/>
+    </row>
+    <row r="24" spans="1:6" s="18" customFormat="1" ht="12">
+      <c r="A24" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A25" s="8">
         <v>4</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B25" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C25" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="15"/>
-      <c r="F22" s="18"/>
-    </row>
-    <row r="23" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A23" s="11">
-        <v>2</v>
-      </c>
-      <c r="B23" s="11" t="s">
+      <c r="D25" s="11"/>
+      <c r="F25" s="13"/>
+    </row>
+    <row r="26" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A26" s="8">
+        <v>2</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C26" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="18"/>
-    </row>
-    <row r="24" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A24" s="11">
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A27" s="8">
         <v>6</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B27" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C27" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="F24" s="18"/>
-    </row>
-    <row r="25" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A25" s="11">
-        <v>2</v>
-      </c>
-      <c r="B25" s="11" t="s">
+      <c r="D27" s="11"/>
+      <c r="F27" s="13"/>
+    </row>
+    <row r="28" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A28" s="8">
+        <v>2</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C28" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="18"/>
-    </row>
-    <row r="26" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A26" s="11">
-        <v>2</v>
-      </c>
-      <c r="B26" s="11" t="s">
+      <c r="F28" s="13"/>
+    </row>
+    <row r="29" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A29" s="8">
+        <v>2</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C29" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F26" s="18"/>
-    </row>
-    <row r="27" spans="1:6" s="14" customFormat="1" ht="12">
-      <c r="A27" s="16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A28" s="11">
+      <c r="F29" s="13"/>
+    </row>
+    <row r="30" spans="1:6" s="18" customFormat="1" ht="12">
+      <c r="A30" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A31" s="8">
         <v>10</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B31" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C31" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="18"/>
-    </row>
-    <row r="29" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A29" s="11">
+      <c r="F31" s="13"/>
+    </row>
+    <row r="32" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A32" s="8">
         <v>10</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B32" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C32" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="18"/>
-    </row>
-    <row r="30" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A30" s="11">
+      <c r="F32" s="13"/>
+    </row>
+    <row r="33" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A33" s="8">
         <v>10</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B33" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C33" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="18"/>
-    </row>
-    <row r="31" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A31" s="11">
+      <c r="F33" s="13"/>
+    </row>
+    <row r="34" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A34" s="8">
         <v>20</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B34" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C34" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="18"/>
-    </row>
-    <row r="32" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A32" s="11">
+      <c r="F34" s="13"/>
+    </row>
+    <row r="35" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A35" s="8">
         <v>10</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B35" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C35" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="18"/>
-    </row>
-    <row r="33" spans="1:6" s="13" customFormat="1" ht="12">
-      <c r="A33" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A34" s="11">
+      <c r="F35" s="13"/>
+    </row>
+    <row r="36" spans="1:6" s="16" customFormat="1" ht="12">
+      <c r="A36" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A37" s="8">
         <v>10</v>
       </c>
-      <c r="B34" s="11">
+      <c r="B37" s="8">
         <v>100</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C37" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F34" s="18"/>
-    </row>
-    <row r="35" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A35" s="11">
+      <c r="F37" s="13"/>
+    </row>
+    <row r="38" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A38" s="8">
         <v>10</v>
       </c>
-      <c r="B35" s="11">
+      <c r="B38" s="8">
         <v>270</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C38" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F35" s="18"/>
-    </row>
-    <row r="36" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A36" s="11">
+      <c r="F38" s="13"/>
+    </row>
+    <row r="39" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A39" s="8">
         <v>10</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B39" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C39" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F36" s="18"/>
-    </row>
-    <row r="37" spans="1:6" s="13" customFormat="1" ht="12">
-      <c r="A37" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A38" s="11">
+      <c r="F39" s="13"/>
+    </row>
+    <row r="40" spans="1:6" s="16" customFormat="1" ht="12">
+      <c r="A40" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A41" s="8">
         <v>20</v>
       </c>
-      <c r="B38" s="11">
-        <v>2</v>
-      </c>
-      <c r="C38" s="12" t="s">
+      <c r="B41" s="8">
+        <v>2</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F38" s="18"/>
-    </row>
-    <row r="39" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A39" s="11">
+      <c r="F41" s="13"/>
+    </row>
+    <row r="42" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A42" s="8">
         <v>10</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B42" s="8">
         <v>3.3</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C42" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F39" s="18"/>
-    </row>
-    <row r="40" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A40" s="11">
+      <c r="F42" s="13"/>
+    </row>
+    <row r="43" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A43" s="8">
         <v>10</v>
       </c>
-      <c r="B40" s="11">
+      <c r="B43" s="8">
         <v>10</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C43" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F40" s="18"/>
-    </row>
-    <row r="41" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A41" s="11">
+      <c r="F43" s="13"/>
+    </row>
+    <row r="44" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A44" s="8">
         <v>10</v>
       </c>
-      <c r="B41" s="11">
+      <c r="B44" s="8">
         <v>51</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C44" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F41" s="18"/>
-    </row>
-    <row r="42" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A42" s="11">
+      <c r="F44" s="13"/>
+    </row>
+    <row r="45" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A45" s="8">
         <v>10</v>
       </c>
-      <c r="B42" s="11">
+      <c r="B45" s="8">
         <v>510</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C45" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F42" s="18"/>
-    </row>
-    <row r="43" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A43" s="11">
+      <c r="F45" s="13"/>
+    </row>
+    <row r="46" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A46" s="8">
         <v>10</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B46" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C46" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F43" s="18"/>
-    </row>
-    <row r="44" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A44" s="11">
+      <c r="F46" s="13"/>
+    </row>
+    <row r="47" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A47" s="8">
         <v>10</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B47" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C47" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F44" s="18"/>
-    </row>
-    <row r="45" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A45" s="11">
+      <c r="F47" s="13"/>
+    </row>
+    <row r="48" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A48" s="8">
         <v>10</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B48" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C48" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F45" s="18"/>
-    </row>
-    <row r="46" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A46" s="11">
+      <c r="F48" s="13"/>
+    </row>
+    <row r="49" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A49" s="8">
         <v>10</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B49" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C49" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F46" s="18"/>
-    </row>
-    <row r="47" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A47" s="11">
+      <c r="F49" s="13"/>
+    </row>
+    <row r="50" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A50" s="8">
         <v>10</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B50" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C50" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F47" s="18"/>
-    </row>
-    <row r="48" spans="1:6" s="13" customFormat="1" ht="12">
-      <c r="A48" s="17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A49" s="11">
-        <v>2</v>
-      </c>
-      <c r="B49" s="11" t="s">
+      <c r="F50" s="13"/>
+    </row>
+    <row r="51" spans="1:6" s="16" customFormat="1" ht="12">
+      <c r="A51" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A52" s="8">
+        <v>2</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C52" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F49" s="18"/>
-    </row>
-    <row r="50" spans="1:6" s="13" customFormat="1" ht="12">
-      <c r="A50" s="17" t="s">
+      <c r="F52" s="13"/>
+    </row>
+    <row r="53" spans="1:6" s="16" customFormat="1" ht="12">
+      <c r="A53" s="15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A51" s="11">
+    <row r="54" spans="1:6" s="10" customFormat="1" ht="12">
+      <c r="A54" s="8">
+        <v>2</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F54" s="26"/>
+    </row>
+    <row r="55" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A55" s="8">
         <v>17</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B55" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C55" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F51" s="18"/>
-    </row>
-    <row r="52" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A52" s="11">
-        <v>1</v>
-      </c>
-      <c r="B52" s="11" t="s">
+      <c r="F55" s="13"/>
+    </row>
+    <row r="56" spans="1:6" s="9" customFormat="1" ht="12">
+      <c r="A56" s="8">
+        <v>1</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C56" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F52" s="18"/>
+      <c r="F56" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A33:XFD33"/>
-    <mergeCell ref="A37:XFD37"/>
-    <mergeCell ref="A48:XFD48"/>
-    <mergeCell ref="A50:XFD50"/>
-    <mergeCell ref="A2:XFD2"/>
-    <mergeCell ref="A9:XFD9"/>
-    <mergeCell ref="A11:XFD11"/>
-    <mergeCell ref="A17:XFD17"/>
-    <mergeCell ref="A21:XFD21"/>
-    <mergeCell ref="A27:XFD27"/>
+    <mergeCell ref="A36:XFD36"/>
+    <mergeCell ref="A40:XFD40"/>
+    <mergeCell ref="A51:XFD51"/>
+    <mergeCell ref="A53:XFD53"/>
+    <mergeCell ref="A5:XFD5"/>
+    <mergeCell ref="A12:XFD12"/>
+    <mergeCell ref="A14:XFD14"/>
+    <mergeCell ref="A20:XFD20"/>
+    <mergeCell ref="A24:XFD24"/>
+    <mergeCell ref="A30:XFD30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1370,23 +1446,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="5" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" s="21" customFormat="1">
+      <c r="A1" s="21" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1397,10 +1473,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="2" customFormat="1">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1411,10 +1487,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" s="2" customFormat="1">
-      <c r="A4" s="7">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1425,10 +1501,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" s="2" customFormat="1">
-      <c r="A5" s="7">
-        <v>1</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1439,10 +1515,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1">
-      <c r="A6" s="7">
-        <v>1</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1453,10 +1529,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1">
-      <c r="A7" s="7">
-        <v>2</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="4">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1466,32 +1542,32 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:4" s="19" customFormat="1">
+      <c r="A8" s="19" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="2" customFormat="1">
-      <c r="A9" s="7">
-        <v>1</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="4">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="6" customFormat="1">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:4" s="20" customFormat="1">
+      <c r="A10" s="20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="2" customFormat="1">
-      <c r="A11" s="7">
-        <v>2</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="4">
+        <v>2</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1499,10 +1575,10 @@
       </c>
     </row>
     <row r="12" spans="1:4" s="2" customFormat="1">
-      <c r="A12" s="7">
-        <v>1</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="4">
+        <v>1</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1510,10 +1586,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" s="2" customFormat="1">
-      <c r="A13" s="7">
-        <v>2</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="4">
+        <v>2</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1521,10 +1597,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" s="2" customFormat="1">
-      <c r="A14" s="7">
-        <v>2</v>
-      </c>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="4">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1532,55 +1608,55 @@
       </c>
     </row>
     <row r="15" spans="1:4" s="2" customFormat="1">
-      <c r="A15" s="7">
-        <v>2</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="4">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="6" customFormat="1">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:4" s="20" customFormat="1">
+      <c r="A16" s="20" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="2" customFormat="1">
-      <c r="A17" s="7">
-        <v>2</v>
-      </c>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="4">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="2" customFormat="1">
-      <c r="A18" s="7">
-        <v>2</v>
-      </c>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="4">
+        <v>2</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="2" customFormat="1">
-      <c r="A19" s="7">
-        <v>1</v>
-      </c>
-      <c r="B19" s="7" t="s">
+      <c r="A19" s="4">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="6" customFormat="1">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:4" s="20" customFormat="1">
+      <c r="A20" s="20" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="2" customFormat="1">
-      <c r="A21" s="7">
-        <v>1</v>
-      </c>
-      <c r="B21" s="7" t="s">
+      <c r="A21" s="4">
+        <v>1</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1588,10 +1664,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" s="2" customFormat="1">
-      <c r="A22" s="7">
-        <v>1</v>
-      </c>
-      <c r="B22" s="7" t="s">
+      <c r="A22" s="4">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1599,10 +1675,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" s="2" customFormat="1">
-      <c r="A23" s="7">
+      <c r="A23" s="4">
         <v>3</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1611,10 +1687,10 @@
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" s="2" customFormat="1">
-      <c r="A24" s="7">
-        <v>2</v>
-      </c>
-      <c r="B24" s="7" t="s">
+      <c r="A24" s="4">
+        <v>2</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1623,26 +1699,26 @@
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" s="2" customFormat="1">
-      <c r="A25" s="7">
-        <v>1</v>
-      </c>
-      <c r="B25" s="7" t="s">
+      <c r="A25" s="4">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="6" customFormat="1">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:4" s="20" customFormat="1">
+      <c r="A26" s="20" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="2" customFormat="1">
-      <c r="A27" s="7">
-        <v>1</v>
-      </c>
-      <c r="B27" s="7" t="s">
+      <c r="A27" s="4">
+        <v>1</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -1650,10 +1726,10 @@
       </c>
     </row>
     <row r="28" spans="1:4" s="2" customFormat="1">
-      <c r="A28" s="7">
-        <v>1</v>
-      </c>
-      <c r="B28" s="7" t="s">
+      <c r="A28" s="4">
+        <v>1</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1661,10 +1737,10 @@
       </c>
     </row>
     <row r="29" spans="1:4" s="2" customFormat="1">
-      <c r="A29" s="7">
+      <c r="A29" s="4">
         <v>7</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1672,10 +1748,10 @@
       </c>
     </row>
     <row r="30" spans="1:4" s="2" customFormat="1">
-      <c r="A30" s="7">
-        <v>1</v>
-      </c>
-      <c r="B30" s="7" t="s">
+      <c r="A30" s="4">
+        <v>1</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -1683,26 +1759,26 @@
       </c>
     </row>
     <row r="31" spans="1:4" s="2" customFormat="1">
-      <c r="A31" s="7">
-        <v>2</v>
-      </c>
-      <c r="B31" s="7" t="s">
+      <c r="A31" s="4">
+        <v>2</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="5" customFormat="1">
-      <c r="A32" s="5" t="s">
+    <row r="32" spans="1:4" s="19" customFormat="1">
+      <c r="A32" s="19" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="2" customFormat="1">
-      <c r="A33" s="7">
-        <v>2</v>
-      </c>
-      <c r="B33" s="7" t="s">
+      <c r="A33" s="4">
+        <v>2</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -1710,10 +1786,10 @@
       </c>
     </row>
     <row r="34" spans="1:3" s="2" customFormat="1">
-      <c r="A34" s="7">
+      <c r="A34" s="4">
         <v>5</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34" s="4">
         <v>270</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -1721,26 +1797,26 @@
       </c>
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1">
-      <c r="A35" s="7">
-        <v>2</v>
-      </c>
-      <c r="B35" s="7">
+      <c r="A35" s="4">
+        <v>2</v>
+      </c>
+      <c r="B35" s="4">
         <v>100</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="5" customFormat="1">
-      <c r="A36" s="5" t="s">
+    <row r="36" spans="1:3" s="19" customFormat="1">
+      <c r="A36" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="2" customFormat="1">
-      <c r="A37" s="7">
-        <v>2</v>
-      </c>
-      <c r="B37" s="7" t="s">
+      <c r="A37" s="4">
+        <v>2</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -1748,10 +1824,10 @@
       </c>
     </row>
     <row r="38" spans="1:3" s="2" customFormat="1">
-      <c r="A38" s="7">
-        <v>1</v>
-      </c>
-      <c r="B38" s="7" t="s">
+      <c r="A38" s="4">
+        <v>1</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -1759,10 +1835,10 @@
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1">
-      <c r="A39" s="7">
+      <c r="A39" s="4">
         <v>5</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -1770,10 +1846,10 @@
       </c>
     </row>
     <row r="40" spans="1:3" s="2" customFormat="1">
-      <c r="A40" s="7">
-        <v>1</v>
-      </c>
-      <c r="B40" s="7" t="s">
+      <c r="A40" s="4">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -1781,10 +1857,10 @@
       </c>
     </row>
     <row r="41" spans="1:3" s="2" customFormat="1">
-      <c r="A41" s="7">
+      <c r="A41" s="4">
         <v>3</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -1792,10 +1868,10 @@
       </c>
     </row>
     <row r="42" spans="1:3" s="2" customFormat="1">
-      <c r="A42" s="7">
-        <v>2</v>
-      </c>
-      <c r="B42" s="7">
+      <c r="A42" s="4">
+        <v>2</v>
+      </c>
+      <c r="B42" s="4">
         <v>510</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -1803,10 +1879,10 @@
       </c>
     </row>
     <row r="43" spans="1:3" s="2" customFormat="1">
-      <c r="A43" s="7">
+      <c r="A43" s="4">
         <v>3</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="4">
         <v>51</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -1814,10 +1890,10 @@
       </c>
     </row>
     <row r="44" spans="1:3" s="2" customFormat="1">
-      <c r="A44" s="7">
+      <c r="A44" s="4">
         <v>3</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="4">
         <v>10</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -1825,10 +1901,10 @@
       </c>
     </row>
     <row r="45" spans="1:3" s="2" customFormat="1">
-      <c r="A45" s="7">
-        <v>1</v>
-      </c>
-      <c r="B45" s="7">
+      <c r="A45" s="4">
+        <v>1</v>
+      </c>
+      <c r="B45" s="4">
         <v>3.3</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -1836,42 +1912,42 @@
       </c>
     </row>
     <row r="46" spans="1:3" s="2" customFormat="1">
-      <c r="A46" s="7">
+      <c r="A46" s="4">
         <v>8</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B46" s="4">
         <v>2</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="5" customFormat="1">
-      <c r="A47" s="5" t="s">
+    <row r="47" spans="1:3" s="19" customFormat="1">
+      <c r="A47" s="19" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="2" customFormat="1">
-      <c r="A48" s="7">
-        <v>1</v>
-      </c>
-      <c r="B48" s="7" t="s">
+      <c r="A48" s="4">
+        <v>1</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="5" customFormat="1">
-      <c r="A49" s="5" t="s">
+    <row r="49" spans="1:3" s="19" customFormat="1">
+      <c r="A49" s="19" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="2" customFormat="1">
-      <c r="A50" s="7">
+      <c r="A50" s="4">
         <v>17</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C50" s="2" t="s">
@@ -1879,10 +1955,10 @@
       </c>
     </row>
     <row r="51" spans="1:3" s="2" customFormat="1">
-      <c r="A51" s="7">
-        <v>1</v>
-      </c>
-      <c r="B51" s="7" t="s">
+      <c r="A51" s="4">
+        <v>1</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C51" s="2" t="s">
@@ -1891,16 +1967,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A49:XFD49"/>
+    <mergeCell ref="A16:XFD16"/>
+    <mergeCell ref="A20:XFD20"/>
+    <mergeCell ref="A26:XFD26"/>
+    <mergeCell ref="A32:XFD32"/>
     <mergeCell ref="A36:XFD36"/>
     <mergeCell ref="A47:XFD47"/>
     <mergeCell ref="A10:XFD10"/>
     <mergeCell ref="A1:XFD1"/>
     <mergeCell ref="A8:XFD8"/>
-    <mergeCell ref="A49:XFD49"/>
-    <mergeCell ref="A16:XFD16"/>
-    <mergeCell ref="A20:XFD20"/>
-    <mergeCell ref="A26:XFD26"/>
-    <mergeCell ref="A32:XFD32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>